<commit_message>
evaluation text 95% now on to the TODOs :)
</commit_message>
<xml_diff>
--- a/finalTests/Testes Finais.xlsx
+++ b/finalTests/Testes Finais.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="701" activeTab="15"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="701" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Unav1" sheetId="6" r:id="rId1"/>
@@ -1860,9 +1860,6 @@
     <t>I successfully used the geometry modeling operations.</t>
   </si>
   <si>
-    <t>The learning curve was confortable.</t>
-  </si>
-  <si>
     <t>The menu invocation and shape feature selection gestures were easy to learn.</t>
   </si>
   <si>
@@ -1970,6 +1967,9 @@
   </si>
   <si>
     <t>after</t>
+  </si>
+  <si>
+    <t>The learning curve was comfortable.</t>
   </si>
 </sst>
 </file>
@@ -1978,7 +1978,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="173" formatCode="00%"/>
+    <numFmt numFmtId="165" formatCode="00%"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -2838,9 +2838,6 @@
     <xf numFmtId="0" fontId="4" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2898,12 +2895,6 @@
     <xf numFmtId="0" fontId="4" fillId="21" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2935,12 +2926,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2952,15 +2937,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2974,9 +2950,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2985,15 +2958,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3024,15 +2988,6 @@
     <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -3051,16 +3006,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3085,15 +3040,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3132,15 +3078,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3155,6 +3092,69 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4523,25 +4523,25 @@
         </c:ser>
         <c:gapWidth val="79"/>
         <c:overlap val="100"/>
-        <c:axId val="90212992"/>
-        <c:axId val="90281472"/>
+        <c:axId val="72296320"/>
+        <c:axId val="72297856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90212992"/>
+        <c:axId val="72296320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90281472"/>
+        <c:crossAx val="72297856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90281472"/>
+        <c:axId val="72297856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4561,7 +4561,7 @@
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90212992"/>
+        <c:crossAx val="72296320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4590,7 +4590,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4714,7 +4714,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4840,7 +4840,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4899,7 +4899,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-5.5512725788632991E-2"/>
-                  <c:y val="1.3888888888888888E-2"/>
+                  <c:y val="1.3888888888888892E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -4977,7 +4977,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5076,7 +5076,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5223,7 +5223,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5368,12 +5368,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="86004096"/>
-        <c:axId val="86005632"/>
+        <c:axId val="72820224"/>
+        <c:axId val="72822144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86004096"/>
+        <c:axId val="72820224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5398,14 +5397,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86005632"/>
+        <c:crossAx val="72822144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86005632"/>
+        <c:axId val="72822144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5431,7 +5430,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86004096"/>
+        <c:crossAx val="72820224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5443,9 +5442,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.70361242344706909"/>
-          <c:y val="0.37482429279673374"/>
-          <c:w val="0.24083202099737533"/>
-          <c:h val="0.16743438320209975"/>
+          <c:y val="0.37482429279673385"/>
+          <c:w val="0.24083202099737536"/>
+          <c:h val="0.1674343832020998"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -5453,7 +5452,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5463,16 +5462,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8743,7 +8742,7 @@
     </row>
     <row r="166" spans="2:9">
       <c r="E166" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F166">
         <f>AVEDEV(H169:H184)</f>
@@ -8764,85 +8763,85 @@
     </row>
     <row r="169" spans="2:9">
       <c r="E169" s="25"/>
-      <c r="G169" s="177"/>
-      <c r="H169" s="175">
+      <c r="G169" s="159"/>
+      <c r="H169" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="170" spans="2:9">
       <c r="E170" s="25"/>
       <c r="G170" s="29"/>
-      <c r="H170" s="175">
+      <c r="H170" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="171" spans="2:9">
-      <c r="H171" s="175">
+      <c r="H171" s="157">
         <v>5</v>
       </c>
     </row>
     <row r="172" spans="2:9">
-      <c r="H172" s="175">
+      <c r="H172" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="173" spans="2:9">
-      <c r="H173" s="175">
+      <c r="H173" s="157">
         <v>5</v>
       </c>
     </row>
     <row r="174" spans="2:9">
-      <c r="H174" s="175">
+      <c r="H174" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="175" spans="2:9">
-      <c r="H175" s="175">
+      <c r="H175" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="176" spans="2:9">
-      <c r="H176" s="175">
+      <c r="H176" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="177" spans="8:8">
-      <c r="H177" s="175">
+      <c r="H177" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="178" spans="8:8">
-      <c r="H178" s="175">
+      <c r="H178" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="179" spans="8:8">
-      <c r="H179" s="175">
+      <c r="H179" s="157">
         <v>4</v>
       </c>
     </row>
     <row r="180" spans="8:8">
-      <c r="H180" s="175">
+      <c r="H180" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="181" spans="8:8">
-      <c r="H181" s="175">
+      <c r="H181" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="182" spans="8:8">
-      <c r="H182" s="175">
+      <c r="H182" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="183" spans="8:8">
-      <c r="H183" s="175">
+      <c r="H183" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="184" spans="8:8">
-      <c r="H184" s="175">
+      <c r="H184" s="157">
         <v>6</v>
       </c>
     </row>
@@ -13748,7 +13747,7 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:23" ht="72">
+    <row r="15" spans="1:23" ht="60">
       <c r="A15" s="48">
         <v>14</v>
       </c>
@@ -13901,19 +13900,19 @@
       <c r="E19" t="s">
         <v>261</v>
       </c>
-      <c r="F19" s="132" t="s">
+      <c r="F19" s="120" t="s">
         <v>270</v>
       </c>
-      <c r="G19" s="129" t="s">
+      <c r="G19" s="117" t="s">
         <v>351</v>
       </c>
-      <c r="H19" s="132" t="s">
+      <c r="H19" s="120" t="s">
         <v>273</v>
       </c>
-      <c r="I19" s="132" t="s">
+      <c r="I19" s="120" t="s">
         <v>279</v>
       </c>
-      <c r="K19" s="130" t="s">
+      <c r="K19" s="118" t="s">
         <v>280</v>
       </c>
     </row>
@@ -13944,7 +13943,7 @@
         <f>12/16</f>
         <v>0.75</v>
       </c>
-      <c r="J20" s="136" t="s">
+      <c r="J20" s="124" t="s">
         <v>282</v>
       </c>
       <c r="K20" s="29">
@@ -13953,16 +13952,16 @@
       </c>
     </row>
     <row r="21" spans="1:23">
-      <c r="F21" s="135" t="s">
+      <c r="F21" s="123" t="s">
         <v>271</v>
       </c>
-      <c r="G21" s="131" t="s">
+      <c r="G21" s="119" t="s">
         <v>352</v>
       </c>
-      <c r="H21" s="137" t="s">
+      <c r="H21" s="125" t="s">
         <v>275</v>
       </c>
-      <c r="I21" s="135" t="s">
+      <c r="I21" s="123" t="s">
         <v>355</v>
       </c>
       <c r="J21" s="29">
@@ -13997,7 +13996,7 @@
         <f>4/16</f>
         <v>0.25</v>
       </c>
-      <c r="J22" s="138" t="s">
+      <c r="J22" s="126" t="s">
         <v>251</v>
       </c>
     </row>
@@ -14012,10 +14011,10 @@
       <c r="F23" s="67" t="s">
         <v>272</v>
       </c>
-      <c r="G23" s="133" t="s">
+      <c r="G23" s="121" t="s">
         <v>354</v>
       </c>
-      <c r="H23" s="133" t="s">
+      <c r="H23" s="121" t="s">
         <v>274</v>
       </c>
       <c r="J23" s="29">
@@ -14043,7 +14042,7 @@
         <f>1/16</f>
         <v>6.25E-2</v>
       </c>
-      <c r="J24" s="134" t="s">
+      <c r="J24" s="122" t="s">
         <v>283</v>
       </c>
     </row>
@@ -14063,7 +14062,7 @@
       <c r="D26">
         <v>7</v>
       </c>
-      <c r="J26" s="131" t="s">
+      <c r="J26" s="119" t="s">
         <v>281</v>
       </c>
     </row>
@@ -14105,23 +14104,23 @@
       </c>
     </row>
     <row r="31" spans="1:23">
-      <c r="F31" s="128">
+      <c r="F31" s="116">
         <f>SUM(F20,F22,F24)</f>
         <v>1</v>
       </c>
-      <c r="G31" s="128">
+      <c r="G31" s="116">
         <f>SUM(G20,G22,G24)</f>
         <v>1</v>
       </c>
-      <c r="H31" s="128">
+      <c r="H31" s="116">
         <f>SUM(H20,H22,H24)</f>
         <v>1</v>
       </c>
-      <c r="I31" s="128">
+      <c r="I31" s="116">
         <f>SUM(I20,I22,I24,I26)</f>
         <v>1</v>
       </c>
-      <c r="J31" s="128">
+      <c r="J31" s="116">
         <f>SUM(J27,J21,J25,J23)</f>
         <v>1</v>
       </c>
@@ -14179,190 +14178,190 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="68"/>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="170" t="s">
         <v>347</v>
       </c>
-      <c r="C3" s="179" t="s">
+      <c r="C3" s="175" t="s">
         <v>313</v>
       </c>
-      <c r="D3" s="180"/>
-      <c r="E3" s="180"/>
-      <c r="F3" s="181"/>
-      <c r="G3" s="179" t="s">
+      <c r="D3" s="176"/>
+      <c r="E3" s="176"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="175" t="s">
         <v>314</v>
       </c>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="76" t="s">
+      <c r="H3" s="176"/>
+      <c r="I3" s="176"/>
+      <c r="J3" s="177"/>
+      <c r="K3" s="75" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="68"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="76" t="s">
+      <c r="B4" s="171"/>
+      <c r="C4" s="75" t="s">
         <v>345</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="75" t="s">
         <v>233</v>
       </c>
-      <c r="E4" s="76" t="s">
-        <v>395</v>
-      </c>
-      <c r="F4" s="76" t="s">
+      <c r="E4" s="75" t="s">
+        <v>394</v>
+      </c>
+      <c r="F4" s="75" t="s">
         <v>346</v>
       </c>
-      <c r="G4" s="76" t="s">
+      <c r="G4" s="75" t="s">
         <v>345</v>
       </c>
-      <c r="H4" s="76" t="s">
+      <c r="H4" s="75" t="s">
         <v>233</v>
       </c>
-      <c r="I4" s="76" t="s">
-        <v>395</v>
-      </c>
-      <c r="J4" s="76" t="s">
+      <c r="I4" s="75" t="s">
+        <v>394</v>
+      </c>
+      <c r="J4" s="75" t="s">
         <v>346</v>
       </c>
-      <c r="K4" s="76" t="s">
+      <c r="K4" s="75" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="78" t="s">
         <v>308</v>
       </c>
-      <c r="C5" s="80">
-        <v>1</v>
-      </c>
-      <c r="D5" s="81">
+      <c r="C5" s="79">
+        <v>1</v>
+      </c>
+      <c r="D5" s="80">
         <v>2.75</v>
       </c>
-      <c r="E5" s="185">
+      <c r="E5" s="164">
         <v>1.28125</v>
       </c>
-      <c r="F5" s="82">
+      <c r="F5" s="81">
         <v>6</v>
       </c>
-      <c r="G5" s="80">
-        <v>1</v>
-      </c>
-      <c r="H5" s="81">
+      <c r="G5" s="79">
+        <v>1</v>
+      </c>
+      <c r="H5" s="80">
         <v>1.3752</v>
       </c>
-      <c r="I5" s="185">
+      <c r="I5" s="164">
         <v>0.46875</v>
       </c>
-      <c r="J5" s="82">
-        <v>2</v>
-      </c>
-      <c r="K5" s="172">
+      <c r="J5" s="81">
+        <v>2</v>
+      </c>
+      <c r="K5" s="154">
         <f>(D5-H5)/MAX(D5,H5)</f>
         <v>0.49992727272727272</v>
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="82" t="s">
         <v>309</v>
       </c>
-      <c r="C6" s="84">
-        <v>1</v>
-      </c>
-      <c r="D6" s="85">
+      <c r="C6" s="83">
+        <v>1</v>
+      </c>
+      <c r="D6" s="84">
         <v>1.875</v>
       </c>
-      <c r="E6" s="186">
+      <c r="E6" s="165">
         <v>0.65625</v>
       </c>
-      <c r="F6" s="86">
+      <c r="F6" s="85">
         <v>5</v>
       </c>
-      <c r="G6" s="87">
-        <v>1</v>
-      </c>
-      <c r="H6" s="88">
+      <c r="G6" s="86">
+        <v>1</v>
+      </c>
+      <c r="H6" s="87">
         <v>1.125</v>
       </c>
-      <c r="I6" s="186">
+      <c r="I6" s="165">
         <v>0.15277777777777771</v>
       </c>
-      <c r="J6" s="86">
-        <v>2</v>
-      </c>
-      <c r="K6" s="173">
+      <c r="J6" s="85">
+        <v>2</v>
+      </c>
+      <c r="K6" s="155">
         <f>(D6-H6)/MAX(D6,H6)</f>
         <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="82" t="s">
         <v>310</v>
       </c>
-      <c r="C7" s="84">
-        <v>1</v>
-      </c>
-      <c r="D7" s="85">
+      <c r="C7" s="83">
+        <v>1</v>
+      </c>
+      <c r="D7" s="84">
         <v>6.0625</v>
       </c>
-      <c r="E7" s="186">
+      <c r="E7" s="165">
         <v>1.5703125</v>
       </c>
-      <c r="F7" s="86">
+      <c r="F7" s="85">
         <v>9</v>
       </c>
-      <c r="G7" s="87">
-        <v>1</v>
-      </c>
-      <c r="H7" s="88">
+      <c r="G7" s="86">
+        <v>1</v>
+      </c>
+      <c r="H7" s="87">
         <v>4.375</v>
       </c>
-      <c r="I7" s="182">
+      <c r="I7" s="161">
         <v>0.7109375</v>
       </c>
-      <c r="J7" s="86">
+      <c r="J7" s="85">
         <v>6</v>
       </c>
-      <c r="K7" s="173">
+      <c r="K7" s="155">
         <f>(D7-H7)/MAX(D7,H7)</f>
         <v>0.27835051546391754</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="B8" s="94" t="s">
+      <c r="B8" s="93" t="s">
         <v>311</v>
       </c>
-      <c r="C8" s="89">
-        <v>2</v>
-      </c>
-      <c r="D8" s="90">
+      <c r="C8" s="88">
+        <v>2</v>
+      </c>
+      <c r="D8" s="89">
         <v>5</v>
       </c>
-      <c r="E8" s="182">
+      <c r="E8" s="161">
         <v>1.875</v>
       </c>
-      <c r="F8" s="91">
+      <c r="F8" s="90">
         <v>10</v>
       </c>
-      <c r="G8" s="92">
-        <v>1</v>
-      </c>
-      <c r="H8" s="93">
+      <c r="G8" s="91">
+        <v>1</v>
+      </c>
+      <c r="H8" s="92">
         <v>3.25</v>
       </c>
-      <c r="I8" s="184">
+      <c r="I8" s="163">
         <v>1.96875</v>
       </c>
-      <c r="J8" s="91">
-        <v>8</v>
-      </c>
-      <c r="K8" s="174">
+      <c r="J8" s="90">
+        <v>8</v>
+      </c>
+      <c r="K8" s="156">
         <f>(D8-H8)/MAX(D8,H8)</f>
         <v>0.35</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="77" t="s">
         <v>312</v>
       </c>
       <c r="C9" s="72">
@@ -14371,19 +14370,19 @@
       <c r="D9" s="73">
         <v>3</v>
       </c>
-      <c r="E9" s="183">
+      <c r="E9" s="162">
         <v>1.125</v>
       </c>
       <c r="F9" s="70">
         <v>6</v>
       </c>
-      <c r="G9" s="160" t="s">
+      <c r="G9" s="172" t="s">
         <v>317</v>
       </c>
-      <c r="H9" s="161"/>
-      <c r="I9" s="161"/>
-      <c r="J9" s="162"/>
-      <c r="K9" s="163" t="s">
+      <c r="H9" s="173"/>
+      <c r="I9" s="173"/>
+      <c r="J9" s="174"/>
+      <c r="K9" s="145" t="s">
         <v>318</v>
       </c>
     </row>
@@ -14397,7 +14396,7 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="M12" s="77" t="s">
+      <c r="M12" s="76" t="s">
         <v>328</v>
       </c>
       <c r="N12" s="74" t="s">
@@ -14408,129 +14407,129 @@
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="M13" s="79" t="s">
+      <c r="M13" s="78" t="s">
         <v>308</v>
       </c>
-      <c r="N13" s="100" t="s">
+      <c r="N13" s="97" t="s">
         <v>319</v>
       </c>
-      <c r="O13" s="97">
+      <c r="O13" s="94">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="M14" s="108" t="s">
+      <c r="M14" s="166" t="s">
         <v>309</v>
       </c>
-      <c r="N14" s="110" t="s">
+      <c r="N14" s="105" t="s">
         <v>320</v>
       </c>
-      <c r="O14" s="111">
+      <c r="O14" s="106">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="L15" s="68"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="112" t="s">
+      <c r="M15" s="168"/>
+      <c r="N15" s="107" t="s">
         <v>321</v>
       </c>
-      <c r="O15" s="99">
+      <c r="O15" s="96">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="L16" s="68"/>
-      <c r="M16" s="108" t="s">
+      <c r="M16" s="166" t="s">
         <v>310</v>
       </c>
-      <c r="N16" s="101" t="s">
+      <c r="N16" s="98" t="s">
         <v>321</v>
       </c>
-      <c r="O16" s="98">
+      <c r="O16" s="95">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="12:15">
       <c r="L17" s="68"/>
-      <c r="M17" s="95"/>
-      <c r="N17" s="102" t="s">
+      <c r="M17" s="167"/>
+      <c r="N17" s="99" t="s">
         <v>344</v>
       </c>
-      <c r="O17" s="98">
+      <c r="O17" s="95">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="12:15">
       <c r="L18" s="68"/>
-      <c r="M18" s="95"/>
-      <c r="N18" s="102" t="s">
+      <c r="M18" s="167"/>
+      <c r="N18" s="99" t="s">
         <v>323</v>
       </c>
-      <c r="O18" s="98">
+      <c r="O18" s="95">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="12:15">
       <c r="L19" s="68"/>
-      <c r="M19" s="96"/>
-      <c r="N19" s="103" t="s">
+      <c r="M19" s="168"/>
+      <c r="N19" s="100" t="s">
         <v>324</v>
       </c>
-      <c r="O19" s="99">
+      <c r="O19" s="96">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="12:15">
       <c r="L20" s="68"/>
-      <c r="M20" s="108" t="s">
+      <c r="M20" s="166" t="s">
         <v>311</v>
       </c>
-      <c r="N20" s="102" t="s">
+      <c r="N20" s="99" t="s">
         <v>344</v>
       </c>
-      <c r="O20" s="98">
+      <c r="O20" s="95">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="12:15">
       <c r="L21" s="68"/>
-      <c r="M21" s="96"/>
-      <c r="N21" s="103" t="s">
+      <c r="M21" s="168"/>
+      <c r="N21" s="100" t="s">
         <v>323</v>
       </c>
-      <c r="O21" s="99">
+      <c r="O21" s="96">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="12:15">
       <c r="L22" s="68"/>
-      <c r="M22" s="108" t="s">
+      <c r="M22" s="166" t="s">
         <v>312</v>
       </c>
-      <c r="N22" s="102" t="s">
+      <c r="N22" s="99" t="s">
         <v>344</v>
       </c>
-      <c r="O22" s="98">
+      <c r="O22" s="95">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="12:15">
       <c r="L23" s="68"/>
-      <c r="M23" s="95"/>
-      <c r="N23" s="102" t="s">
+      <c r="M23" s="167"/>
+      <c r="N23" s="99" t="s">
         <v>325</v>
       </c>
-      <c r="O23" s="104">
+      <c r="O23" s="101">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="12:15">
-      <c r="M24" s="109"/>
-      <c r="N24" s="106" t="s">
+      <c r="M24" s="169"/>
+      <c r="N24" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="O24" s="107">
+      <c r="O24" s="104">
         <v>1</v>
       </c>
     </row>
@@ -14557,7 +14556,7 @@
   <dimension ref="B2:Q21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14577,27 +14576,27 @@
       </c>
     </row>
     <row r="3" spans="2:17" ht="28.5" customHeight="1">
-      <c r="B3" s="113"/>
-      <c r="C3" s="113" t="s">
+      <c r="B3" s="108"/>
+      <c r="C3" s="108" t="s">
         <v>343</v>
       </c>
-      <c r="D3" s="113" t="s">
+      <c r="D3" s="108" t="s">
         <v>331</v>
       </c>
-      <c r="E3" s="113" t="s">
+      <c r="E3" s="108" t="s">
         <v>329</v>
       </c>
-      <c r="F3" s="113" t="s">
-        <v>394</v>
+      <c r="F3" s="108" t="s">
+        <v>393</v>
       </c>
       <c r="J3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K3" t="s">
         <v>263</v>
       </c>
       <c r="L3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M3" t="s">
         <v>231</v>
@@ -14606,39 +14605,39 @@
         <v>232</v>
       </c>
       <c r="O3" t="s">
+        <v>420</v>
+      </c>
+      <c r="P3" t="s">
         <v>421</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>422</v>
       </c>
-      <c r="Q3" t="s">
-        <v>423</v>
-      </c>
     </row>
     <row r="4" spans="2:17">
-      <c r="B4" s="114" t="s">
+      <c r="B4" s="178" t="s">
         <v>332</v>
       </c>
-      <c r="C4" s="117" t="s">
+      <c r="C4" s="109" t="s">
         <v>342</v>
       </c>
-      <c r="D4" s="152" t="s">
+      <c r="D4" s="137" t="s">
         <v>376</v>
       </c>
-      <c r="E4" s="156">
+      <c r="E4" s="141">
         <v>3.5</v>
       </c>
-      <c r="F4" s="164">
-        <v>2</v>
-      </c>
-      <c r="G4" s="170"/>
-      <c r="J4" s="117" t="s">
-        <v>401</v>
-      </c>
-      <c r="K4" s="156">
+      <c r="F4" s="146">
+        <v>2</v>
+      </c>
+      <c r="G4" s="152"/>
+      <c r="J4" s="109" t="s">
+        <v>400</v>
+      </c>
+      <c r="K4" s="141">
         <v>3.5</v>
       </c>
-      <c r="L4" s="164">
+      <c r="L4" s="146">
         <v>2</v>
       </c>
       <c r="M4" s="51">
@@ -14663,27 +14662,27 @@
       </c>
     </row>
     <row r="5" spans="2:17">
-      <c r="B5" s="115"/>
-      <c r="C5" s="118" t="s">
+      <c r="B5" s="179"/>
+      <c r="C5" s="110" t="s">
         <v>341</v>
       </c>
-      <c r="D5" s="153" t="s">
+      <c r="D5" s="138" t="s">
         <v>377</v>
       </c>
-      <c r="E5" s="157">
-        <v>2</v>
-      </c>
-      <c r="F5" s="165">
+      <c r="E5" s="142">
+        <v>2</v>
+      </c>
+      <c r="F5" s="147">
         <v>1.125</v>
       </c>
       <c r="G5" s="51"/>
-      <c r="J5" s="118" t="s">
-        <v>402</v>
-      </c>
-      <c r="K5" s="157">
-        <v>2</v>
-      </c>
-      <c r="L5" s="165">
+      <c r="J5" s="110" t="s">
+        <v>401</v>
+      </c>
+      <c r="K5" s="142">
+        <v>2</v>
+      </c>
+      <c r="L5" s="147">
         <v>1.125</v>
       </c>
       <c r="M5" s="51">
@@ -14708,27 +14707,27 @@
       </c>
     </row>
     <row r="6" spans="2:17">
-      <c r="B6" s="115"/>
-      <c r="C6" s="118" t="s">
+      <c r="B6" s="179"/>
+      <c r="C6" s="110" t="s">
         <v>340</v>
       </c>
-      <c r="D6" s="153" t="s">
+      <c r="D6" s="138" t="s">
         <v>378</v>
       </c>
-      <c r="E6" s="157">
-        <v>2</v>
-      </c>
-      <c r="F6" s="165">
+      <c r="E6" s="142">
+        <v>2</v>
+      </c>
+      <c r="F6" s="147">
         <v>0.875</v>
       </c>
-      <c r="G6" s="171"/>
-      <c r="J6" s="118" t="s">
-        <v>403</v>
-      </c>
-      <c r="K6" s="157">
-        <v>2</v>
-      </c>
-      <c r="L6" s="165">
+      <c r="G6" s="153"/>
+      <c r="J6" s="110" t="s">
+        <v>402</v>
+      </c>
+      <c r="K6" s="142">
+        <v>2</v>
+      </c>
+      <c r="L6" s="147">
         <v>0.875</v>
       </c>
       <c r="M6" s="51">
@@ -14753,27 +14752,27 @@
       </c>
     </row>
     <row r="7" spans="2:17">
-      <c r="B7" s="115"/>
-      <c r="C7" s="118" t="s">
+      <c r="B7" s="179"/>
+      <c r="C7" s="110" t="s">
         <v>339</v>
       </c>
-      <c r="D7" s="154" t="s">
+      <c r="D7" s="139" t="s">
         <v>379</v>
       </c>
-      <c r="E7" s="157">
-        <v>2</v>
-      </c>
-      <c r="F7" s="165">
+      <c r="E7" s="142">
+        <v>2</v>
+      </c>
+      <c r="F7" s="147">
         <v>1</v>
       </c>
       <c r="G7" s="51"/>
-      <c r="J7" s="118" t="s">
-        <v>404</v>
-      </c>
-      <c r="K7" s="157">
-        <v>2</v>
-      </c>
-      <c r="L7" s="165">
+      <c r="J7" s="110" t="s">
+        <v>403</v>
+      </c>
+      <c r="K7" s="142">
+        <v>2</v>
+      </c>
+      <c r="L7" s="147">
         <v>1</v>
       </c>
       <c r="M7" s="51">
@@ -14798,27 +14797,27 @@
       </c>
     </row>
     <row r="8" spans="2:17" ht="15" customHeight="1">
-      <c r="B8" s="116"/>
-      <c r="C8" s="120" t="s">
+      <c r="B8" s="180"/>
+      <c r="C8" s="112" t="s">
         <v>338</v>
       </c>
-      <c r="D8" s="155" t="s">
+      <c r="D8" s="140" t="s">
         <v>380</v>
       </c>
-      <c r="E8" s="158">
+      <c r="E8" s="143">
         <v>2.9375</v>
       </c>
-      <c r="F8" s="166">
+      <c r="F8" s="148">
         <v>1.3125</v>
       </c>
       <c r="G8" s="51"/>
-      <c r="J8" s="120" t="s">
-        <v>405</v>
-      </c>
-      <c r="K8" s="158">
+      <c r="J8" s="112" t="s">
+        <v>404</v>
+      </c>
+      <c r="K8" s="143">
         <v>2.9375</v>
       </c>
-      <c r="L8" s="166">
+      <c r="L8" s="148">
         <v>1.3125</v>
       </c>
       <c r="M8" s="51">
@@ -14843,29 +14842,29 @@
       </c>
     </row>
     <row r="9" spans="2:17">
-      <c r="B9" s="114" t="s">
+      <c r="B9" s="178" t="s">
         <v>333</v>
       </c>
-      <c r="C9" s="119" t="s">
+      <c r="C9" s="111" t="s">
         <v>342</v>
       </c>
-      <c r="D9" s="153" t="s">
+      <c r="D9" s="138" t="s">
         <v>381</v>
       </c>
-      <c r="E9" s="159">
+      <c r="E9" s="144">
         <v>4.1875</v>
       </c>
-      <c r="F9" s="164">
+      <c r="F9" s="146">
         <v>0.859375</v>
       </c>
-      <c r="G9" s="171"/>
-      <c r="J9" s="119" t="s">
-        <v>406</v>
-      </c>
-      <c r="K9" s="159">
+      <c r="G9" s="153"/>
+      <c r="J9" s="111" t="s">
+        <v>405</v>
+      </c>
+      <c r="K9" s="144">
         <v>4.1875</v>
       </c>
-      <c r="L9" s="164">
+      <c r="L9" s="146">
         <v>0.859375</v>
       </c>
       <c r="M9" s="51">
@@ -14890,27 +14889,27 @@
       </c>
     </row>
     <row r="10" spans="2:17">
-      <c r="B10" s="115"/>
-      <c r="C10" s="119" t="s">
+      <c r="B10" s="179"/>
+      <c r="C10" s="111" t="s">
         <v>341</v>
       </c>
-      <c r="D10" s="153" t="s">
+      <c r="D10" s="138" t="s">
         <v>382</v>
       </c>
-      <c r="E10" s="159">
+      <c r="E10" s="144">
         <v>5.3125</v>
       </c>
-      <c r="F10" s="167">
+      <c r="F10" s="149">
         <v>0.515625</v>
       </c>
-      <c r="G10" s="171"/>
-      <c r="J10" s="119" t="s">
-        <v>407</v>
-      </c>
-      <c r="K10" s="159">
+      <c r="G10" s="153"/>
+      <c r="J10" s="111" t="s">
+        <v>406</v>
+      </c>
+      <c r="K10" s="144">
         <v>5.3125</v>
       </c>
-      <c r="L10" s="167">
+      <c r="L10" s="149">
         <v>0.515625</v>
       </c>
       <c r="M10" s="51">
@@ -14935,27 +14934,27 @@
       </c>
     </row>
     <row r="11" spans="2:17" ht="24.75">
-      <c r="B11" s="115"/>
-      <c r="C11" s="119" t="s">
+      <c r="B11" s="179"/>
+      <c r="C11" s="111" t="s">
         <v>340</v>
       </c>
-      <c r="D11" s="153" t="s">
-        <v>390</v>
-      </c>
-      <c r="E11" s="159">
+      <c r="D11" s="138" t="s">
+        <v>389</v>
+      </c>
+      <c r="E11" s="144">
         <v>4.8125</v>
       </c>
-      <c r="F11" s="167">
+      <c r="F11" s="149">
         <v>0.65625</v>
       </c>
-      <c r="G11" s="171"/>
-      <c r="J11" s="119" t="s">
-        <v>408</v>
-      </c>
-      <c r="K11" s="159">
+      <c r="G11" s="153"/>
+      <c r="J11" s="111" t="s">
+        <v>407</v>
+      </c>
+      <c r="K11" s="144">
         <v>4.8125</v>
       </c>
-      <c r="L11" s="167">
+      <c r="L11" s="149">
         <v>0.65625</v>
       </c>
       <c r="M11" s="51">
@@ -14980,27 +14979,27 @@
       </c>
     </row>
     <row r="12" spans="2:17">
-      <c r="B12" s="115"/>
-      <c r="C12" s="119" t="s">
+      <c r="B12" s="179"/>
+      <c r="C12" s="111" t="s">
         <v>339</v>
       </c>
-      <c r="D12" s="153" t="s">
+      <c r="D12" s="138" t="s">
         <v>383</v>
       </c>
-      <c r="E12" s="159">
+      <c r="E12" s="144">
         <v>4.0625</v>
       </c>
-      <c r="F12" s="167">
+      <c r="F12" s="149">
         <v>0.828125</v>
       </c>
-      <c r="G12" s="171"/>
-      <c r="J12" s="119" t="s">
-        <v>409</v>
-      </c>
-      <c r="K12" s="159">
+      <c r="G12" s="153"/>
+      <c r="J12" s="111" t="s">
+        <v>408</v>
+      </c>
+      <c r="K12" s="144">
         <v>4.0625</v>
       </c>
-      <c r="L12" s="167">
+      <c r="L12" s="149">
         <v>0.828125</v>
       </c>
       <c r="M12" s="51">
@@ -15025,27 +15024,27 @@
       </c>
     </row>
     <row r="13" spans="2:17" ht="24.75">
-      <c r="B13" s="115"/>
-      <c r="C13" s="119" t="s">
+      <c r="B13" s="179"/>
+      <c r="C13" s="111" t="s">
         <v>338</v>
       </c>
-      <c r="D13" s="153" t="s">
-        <v>391</v>
-      </c>
-      <c r="E13" s="159">
+      <c r="D13" s="138" t="s">
+        <v>390</v>
+      </c>
+      <c r="E13" s="144">
         <v>4.125</v>
       </c>
-      <c r="F13" s="167">
+      <c r="F13" s="149">
         <v>0.796875</v>
       </c>
-      <c r="G13" s="171"/>
-      <c r="J13" s="119" t="s">
-        <v>410</v>
-      </c>
-      <c r="K13" s="159">
+      <c r="G13" s="153"/>
+      <c r="J13" s="111" t="s">
+        <v>409</v>
+      </c>
+      <c r="K13" s="144">
         <v>4.125</v>
       </c>
-      <c r="L13" s="167">
+      <c r="L13" s="149">
         <v>0.796875</v>
       </c>
       <c r="M13" s="51">
@@ -15070,27 +15069,27 @@
       </c>
     </row>
     <row r="14" spans="2:17" ht="24.75">
-      <c r="B14" s="115"/>
-      <c r="C14" s="119" t="s">
+      <c r="B14" s="179"/>
+      <c r="C14" s="111" t="s">
         <v>337</v>
       </c>
-      <c r="D14" s="153" t="s">
-        <v>392</v>
-      </c>
-      <c r="E14" s="159">
+      <c r="D14" s="138" t="s">
+        <v>391</v>
+      </c>
+      <c r="E14" s="144">
         <v>2.875</v>
       </c>
-      <c r="F14" s="167">
+      <c r="F14" s="149">
         <v>0.90625</v>
       </c>
       <c r="G14" s="51"/>
-      <c r="J14" s="119" t="s">
-        <v>411</v>
-      </c>
-      <c r="K14" s="159">
+      <c r="J14" s="111" t="s">
+        <v>410</v>
+      </c>
+      <c r="K14" s="144">
         <v>2.875</v>
       </c>
-      <c r="L14" s="167">
+      <c r="L14" s="149">
         <v>0.90625</v>
       </c>
       <c r="M14" s="51">
@@ -15115,27 +15114,27 @@
       </c>
     </row>
     <row r="15" spans="2:17">
-      <c r="B15" s="115"/>
-      <c r="C15" s="119" t="s">
+      <c r="B15" s="179"/>
+      <c r="C15" s="111" t="s">
         <v>336</v>
       </c>
-      <c r="D15" s="153" t="s">
+      <c r="D15" s="138" t="s">
         <v>384</v>
       </c>
-      <c r="E15" s="159">
+      <c r="E15" s="144">
         <v>4.75</v>
       </c>
-      <c r="F15" s="167">
+      <c r="F15" s="149">
         <v>1.125</v>
       </c>
       <c r="G15" s="51"/>
-      <c r="J15" s="119" t="s">
-        <v>412</v>
-      </c>
-      <c r="K15" s="159">
+      <c r="J15" s="111" t="s">
+        <v>411</v>
+      </c>
+      <c r="K15" s="144">
         <v>4.75</v>
       </c>
-      <c r="L15" s="167">
+      <c r="L15" s="149">
         <v>1.125</v>
       </c>
       <c r="M15" s="51">
@@ -15160,27 +15159,27 @@
       </c>
     </row>
     <row r="16" spans="2:17">
-      <c r="B16" s="115"/>
-      <c r="C16" s="119" t="s">
+      <c r="B16" s="179"/>
+      <c r="C16" s="111" t="s">
         <v>335</v>
       </c>
-      <c r="D16" s="153" t="s">
+      <c r="D16" s="138" t="s">
         <v>385</v>
       </c>
-      <c r="E16" s="159">
+      <c r="E16" s="144">
         <v>4.5625</v>
       </c>
-      <c r="F16" s="167">
+      <c r="F16" s="149">
         <v>0.9765625</v>
       </c>
       <c r="G16" s="51"/>
-      <c r="J16" s="119" t="s">
-        <v>413</v>
-      </c>
-      <c r="K16" s="159">
+      <c r="J16" s="111" t="s">
+        <v>412</v>
+      </c>
+      <c r="K16" s="144">
         <v>4.5625</v>
       </c>
-      <c r="L16" s="167">
+      <c r="L16" s="149">
         <v>0.9765625</v>
       </c>
       <c r="M16" s="51">
@@ -15205,27 +15204,27 @@
       </c>
     </row>
     <row r="17" spans="2:17" ht="24.75">
-      <c r="B17" s="115"/>
-      <c r="C17" s="119" t="s">
+      <c r="B17" s="179"/>
+      <c r="C17" s="111" t="s">
         <v>334</v>
       </c>
-      <c r="D17" s="153" t="s">
+      <c r="D17" s="138" t="s">
         <v>386</v>
       </c>
-      <c r="E17" s="159">
+      <c r="E17" s="144">
         <v>4.6875</v>
       </c>
-      <c r="F17" s="167">
+      <c r="F17" s="149">
         <v>0.8046875</v>
       </c>
-      <c r="G17" s="171"/>
-      <c r="J17" s="119" t="s">
-        <v>414</v>
-      </c>
-      <c r="K17" s="159">
+      <c r="G17" s="153"/>
+      <c r="J17" s="111" t="s">
+        <v>413</v>
+      </c>
+      <c r="K17" s="144">
         <v>4.6875</v>
       </c>
-      <c r="L17" s="167">
+      <c r="L17" s="149">
         <v>0.8046875</v>
       </c>
       <c r="M17" s="51">
@@ -15250,27 +15249,27 @@
       </c>
     </row>
     <row r="18" spans="2:17" ht="24.75">
-      <c r="B18" s="115"/>
-      <c r="C18" s="119">
+      <c r="B18" s="179"/>
+      <c r="C18" s="111">
         <v>10</v>
       </c>
-      <c r="D18" s="153" t="s">
+      <c r="D18" s="138" t="s">
         <v>387</v>
       </c>
-      <c r="E18" s="159">
+      <c r="E18" s="144">
         <v>3.8125</v>
       </c>
-      <c r="F18" s="167">
+      <c r="F18" s="149">
         <v>0.859375</v>
       </c>
-      <c r="G18" s="171"/>
-      <c r="J18" s="119" t="s">
-        <v>415</v>
-      </c>
-      <c r="K18" s="159">
+      <c r="G18" s="153"/>
+      <c r="J18" s="111" t="s">
+        <v>414</v>
+      </c>
+      <c r="K18" s="144">
         <v>3.8125</v>
       </c>
-      <c r="L18" s="167">
+      <c r="L18" s="149">
         <v>0.859375</v>
       </c>
       <c r="M18" s="51">
@@ -15295,27 +15294,27 @@
       </c>
     </row>
     <row r="19" spans="2:17">
-      <c r="B19" s="115"/>
-      <c r="C19" s="119">
+      <c r="B19" s="179"/>
+      <c r="C19" s="111">
         <v>11</v>
       </c>
-      <c r="D19" s="153" t="s">
-        <v>388</v>
-      </c>
-      <c r="E19" s="159">
+      <c r="D19" s="138" t="s">
+        <v>423</v>
+      </c>
+      <c r="E19" s="144">
         <v>5</v>
       </c>
-      <c r="F19" s="167">
+      <c r="F19" s="149">
         <v>0.625</v>
       </c>
-      <c r="G19" s="171"/>
-      <c r="J19" s="119" t="s">
-        <v>416</v>
-      </c>
-      <c r="K19" s="159">
+      <c r="G19" s="153"/>
+      <c r="J19" s="111" t="s">
+        <v>415</v>
+      </c>
+      <c r="K19" s="144">
         <v>5</v>
       </c>
-      <c r="L19" s="167">
+      <c r="L19" s="149">
         <v>0.625</v>
       </c>
       <c r="M19" s="51">
@@ -15340,27 +15339,27 @@
       </c>
     </row>
     <row r="20" spans="2:17" ht="24.75">
-      <c r="B20" s="115"/>
-      <c r="C20" s="119">
+      <c r="B20" s="179"/>
+      <c r="C20" s="111">
         <v>12</v>
       </c>
-      <c r="D20" s="153" t="s">
-        <v>393</v>
-      </c>
-      <c r="E20" s="159">
+      <c r="D20" s="138" t="s">
+        <v>392</v>
+      </c>
+      <c r="E20" s="144">
         <v>2.8125</v>
       </c>
-      <c r="F20" s="168">
+      <c r="F20" s="150">
         <v>1.109375</v>
       </c>
       <c r="G20" s="51"/>
-      <c r="J20" s="119" t="s">
-        <v>417</v>
-      </c>
-      <c r="K20" s="159">
+      <c r="J20" s="111" t="s">
+        <v>416</v>
+      </c>
+      <c r="K20" s="144">
         <v>2.8125</v>
       </c>
-      <c r="L20" s="168">
+      <c r="L20" s="150">
         <v>1.109375</v>
       </c>
       <c r="M20" s="51">
@@ -15385,27 +15384,27 @@
       </c>
     </row>
     <row r="21" spans="2:17" ht="24.75">
-      <c r="B21" s="116"/>
-      <c r="C21" s="120">
+      <c r="B21" s="180"/>
+      <c r="C21" s="112">
         <v>13</v>
       </c>
-      <c r="D21" s="155" t="s">
-        <v>389</v>
-      </c>
-      <c r="E21" s="158">
+      <c r="D21" s="140" t="s">
+        <v>388</v>
+      </c>
+      <c r="E21" s="143">
         <v>5.1875</v>
       </c>
-      <c r="F21" s="169">
+      <c r="F21" s="151">
         <v>0.609375</v>
       </c>
-      <c r="G21" s="171"/>
-      <c r="J21" s="120" t="s">
-        <v>418</v>
-      </c>
-      <c r="K21" s="158">
+      <c r="G21" s="153"/>
+      <c r="J21" s="112" t="s">
+        <v>417</v>
+      </c>
+      <c r="K21" s="143">
         <v>5.1875</v>
       </c>
-      <c r="L21" s="169">
+      <c r="L21" s="151">
         <v>0.609375</v>
       </c>
       <c r="M21" s="51">
@@ -15462,7 +15461,7 @@
   </sheetPr>
   <dimension ref="B2:F31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -15482,275 +15481,275 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="27.75" customHeight="1">
-      <c r="C4" s="113" t="s">
+      <c r="C4" s="108" t="s">
         <v>348</v>
       </c>
-      <c r="D4" s="113" t="s">
+      <c r="D4" s="108" t="s">
         <v>331</v>
       </c>
-      <c r="E4" s="113" t="s">
+      <c r="E4" s="108" t="s">
         <v>349</v>
       </c>
-      <c r="F4" s="113" t="s">
+      <c r="F4" s="108" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="C5" s="125">
-        <v>1</v>
-      </c>
-      <c r="D5" s="139" t="s">
+      <c r="C5" s="181">
+        <v>1</v>
+      </c>
+      <c r="D5" s="183" t="s">
         <v>375</v>
       </c>
-      <c r="E5" s="122" t="s">
+      <c r="E5" s="113" t="s">
         <v>372</v>
       </c>
-      <c r="F5" s="148">
+      <c r="F5" s="133">
         <f>7/16</f>
         <v>0.4375</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="C6" s="126"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="124" t="s">
+      <c r="C6" s="185"/>
+      <c r="D6" s="186"/>
+      <c r="E6" s="115" t="s">
         <v>358</v>
       </c>
-      <c r="F6" s="149">
+      <c r="F6" s="134">
         <f>7/16</f>
         <v>0.4375</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="C7" s="127"/>
-      <c r="D7" s="141"/>
-      <c r="E7" s="123" t="s">
+      <c r="C7" s="182"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="114" t="s">
         <v>357</v>
       </c>
-      <c r="F7" s="150">
+      <c r="F7" s="135">
         <f>2/16</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="24">
-      <c r="C8" s="125">
-        <v>2</v>
-      </c>
-      <c r="D8" s="139" t="s">
+      <c r="C8" s="181">
+        <v>2</v>
+      </c>
+      <c r="D8" s="183" t="s">
         <v>374</v>
       </c>
-      <c r="E8" s="142" t="s">
+      <c r="E8" s="127" t="s">
         <v>359</v>
       </c>
-      <c r="F8" s="148">
+      <c r="F8" s="133">
         <f>13/16</f>
         <v>0.8125</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="24">
-      <c r="C9" s="126"/>
-      <c r="D9" s="140"/>
-      <c r="E9" s="143" t="s">
+      <c r="C9" s="185"/>
+      <c r="D9" s="186"/>
+      <c r="E9" s="128" t="s">
         <v>362</v>
       </c>
-      <c r="F9" s="149">
+      <c r="F9" s="134">
         <f>2/16</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="C10" s="127"/>
-      <c r="D10" s="141"/>
-      <c r="E10" s="123" t="s">
+      <c r="C10" s="182"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="114" t="s">
         <v>356</v>
       </c>
-      <c r="F10" s="150">
+      <c r="F10" s="135">
         <f>1/16</f>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="C11" s="125">
-        <v>3</v>
-      </c>
-      <c r="D11" s="139" t="s">
+      <c r="C11" s="181">
+        <v>3</v>
+      </c>
+      <c r="D11" s="183" t="s">
         <v>360</v>
       </c>
-      <c r="E11" s="122" t="s">
+      <c r="E11" s="113" t="s">
         <v>370</v>
       </c>
-      <c r="F11" s="148">
+      <c r="F11" s="133">
         <f>12/16</f>
         <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="24">
-      <c r="C12" s="126"/>
-      <c r="D12" s="140"/>
-      <c r="E12" s="144" t="s">
+      <c r="C12" s="185"/>
+      <c r="D12" s="186"/>
+      <c r="E12" s="129" t="s">
         <v>371</v>
       </c>
-      <c r="F12" s="149">
+      <c r="F12" s="134">
         <f>3/16</f>
         <v>0.1875</v>
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="C13" s="127"/>
-      <c r="D13" s="141"/>
-      <c r="E13" s="123" t="s">
+      <c r="C13" s="182"/>
+      <c r="D13" s="184"/>
+      <c r="E13" s="114" t="s">
         <v>361</v>
       </c>
-      <c r="F13" s="150">
+      <c r="F13" s="135">
         <f>1/16</f>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15" customHeight="1">
-      <c r="C14" s="125">
+      <c r="C14" s="181">
         <v>4</v>
       </c>
-      <c r="D14" s="139" t="s">
+      <c r="D14" s="183" t="s">
         <v>363</v>
       </c>
-      <c r="E14" s="122" t="s">
+      <c r="E14" s="113" t="s">
         <v>364</v>
       </c>
-      <c r="F14" s="148">
+      <c r="F14" s="133">
         <f>12/16</f>
         <v>0.75</v>
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="C15" s="127"/>
-      <c r="D15" s="141"/>
-      <c r="E15" s="123" t="s">
+      <c r="C15" s="182"/>
+      <c r="D15" s="184"/>
+      <c r="E15" s="114" t="s">
         <v>365</v>
       </c>
-      <c r="F15" s="150">
+      <c r="F15" s="135">
         <f>4/16</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="15" customHeight="1">
-      <c r="C16" s="125">
+      <c r="C16" s="181">
         <v>5</v>
       </c>
-      <c r="D16" s="139" t="s">
+      <c r="D16" s="183" t="s">
         <v>373</v>
       </c>
-      <c r="E16" s="122" t="s">
+      <c r="E16" s="113" t="s">
         <v>366</v>
       </c>
-      <c r="F16" s="148">
+      <c r="F16" s="133">
         <f>5/16</f>
         <v>0.3125</v>
       </c>
     </row>
     <row r="17" spans="3:6">
-      <c r="C17" s="126"/>
-      <c r="D17" s="140"/>
-      <c r="E17" s="124" t="s">
+      <c r="C17" s="185"/>
+      <c r="D17" s="186"/>
+      <c r="E17" s="115" t="s">
         <v>367</v>
       </c>
-      <c r="F17" s="149">
+      <c r="F17" s="134">
         <f>5/16</f>
         <v>0.3125</v>
       </c>
     </row>
     <row r="18" spans="3:6">
-      <c r="C18" s="126"/>
-      <c r="D18" s="140"/>
-      <c r="E18" s="124" t="s">
+      <c r="C18" s="185"/>
+      <c r="D18" s="186"/>
+      <c r="E18" s="115" t="s">
         <v>368</v>
       </c>
-      <c r="F18" s="151">
+      <c r="F18" s="136">
         <f>4/16</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="19" spans="3:6">
-      <c r="C19" s="127"/>
-      <c r="D19" s="141"/>
-      <c r="E19" s="123" t="s">
+      <c r="C19" s="182"/>
+      <c r="D19" s="184"/>
+      <c r="E19" s="114" t="s">
         <v>369</v>
       </c>
-      <c r="F19" s="150">
+      <c r="F19" s="135">
         <f>2/16</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="20" spans="3:6">
-      <c r="C20" s="147"/>
-      <c r="D20" s="145"/>
-      <c r="E20" s="146"/>
-      <c r="F20" s="105"/>
+      <c r="C20" s="132"/>
+      <c r="D20" s="130"/>
+      <c r="E20" s="131"/>
+      <c r="F20" s="102"/>
     </row>
     <row r="21" spans="3:6">
-      <c r="C21" s="147"/>
-      <c r="D21" s="145"/>
-      <c r="E21" s="146"/>
-      <c r="F21" s="105"/>
+      <c r="C21" s="132"/>
+      <c r="D21" s="130"/>
+      <c r="E21" s="131"/>
+      <c r="F21" s="102"/>
     </row>
     <row r="22" spans="3:6">
-      <c r="C22" s="147"/>
-      <c r="D22" s="145"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="132"/>
+      <c r="D22" s="130"/>
+      <c r="E22" s="131"/>
+      <c r="F22" s="102"/>
     </row>
     <row r="23" spans="3:6">
-      <c r="C23" s="147"/>
-      <c r="D23" s="145"/>
-      <c r="E23" s="146"/>
-      <c r="F23" s="105"/>
+      <c r="C23" s="132"/>
+      <c r="D23" s="130"/>
+      <c r="E23" s="131"/>
+      <c r="F23" s="102"/>
     </row>
     <row r="24" spans="3:6">
-      <c r="C24" s="147"/>
-      <c r="D24" s="145"/>
-      <c r="E24" s="146"/>
-      <c r="F24" s="105"/>
+      <c r="C24" s="132"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="131"/>
+      <c r="F24" s="102"/>
     </row>
     <row r="25" spans="3:6">
-      <c r="C25" s="147"/>
-      <c r="D25" s="145"/>
-      <c r="E25" s="146"/>
-      <c r="F25" s="105"/>
+      <c r="C25" s="132"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="131"/>
+      <c r="F25" s="102"/>
     </row>
     <row r="26" spans="3:6">
-      <c r="C26" s="147"/>
-      <c r="D26" s="145"/>
-      <c r="E26" s="146"/>
-      <c r="F26" s="105"/>
+      <c r="C26" s="132"/>
+      <c r="D26" s="130"/>
+      <c r="E26" s="131"/>
+      <c r="F26" s="102"/>
     </row>
     <row r="27" spans="3:6">
-      <c r="C27" s="147"/>
-      <c r="D27" s="145"/>
-      <c r="E27" s="146"/>
-      <c r="F27" s="105"/>
+      <c r="C27" s="132"/>
+      <c r="D27" s="130"/>
+      <c r="E27" s="131"/>
+      <c r="F27" s="102"/>
     </row>
     <row r="28" spans="3:6">
-      <c r="C28" s="147"/>
-      <c r="D28" s="145"/>
-      <c r="E28" s="146"/>
-      <c r="F28" s="105"/>
+      <c r="C28" s="132"/>
+      <c r="D28" s="130"/>
+      <c r="E28" s="131"/>
+      <c r="F28" s="102"/>
     </row>
     <row r="29" spans="3:6">
-      <c r="C29" s="147"/>
-      <c r="D29" s="145"/>
-      <c r="E29" s="146"/>
-      <c r="F29" s="105"/>
+      <c r="C29" s="132"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="131"/>
+      <c r="F29" s="102"/>
     </row>
     <row r="30" spans="3:6">
-      <c r="C30" s="147"/>
-      <c r="D30" s="145"/>
-      <c r="E30" s="146"/>
-      <c r="F30" s="105"/>
+      <c r="C30" s="132"/>
+      <c r="D30" s="130"/>
+      <c r="E30" s="131"/>
+      <c r="F30" s="102"/>
     </row>
     <row r="31" spans="3:6">
-      <c r="C31" s="105"/>
-      <c r="D31" s="105"/>
-      <c r="E31" s="105"/>
-      <c r="F31" s="105"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="102"/>
+      <c r="F31" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -15774,7 +15773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
@@ -15782,7 +15781,7 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="58" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C2" s="58" t="s">
         <v>313</v>
@@ -15793,45 +15792,45 @@
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="58" t="s">
-        <v>396</v>
-      </c>
-      <c r="C3" s="81">
+        <v>395</v>
+      </c>
+      <c r="C3" s="80">
         <v>2.75</v>
       </c>
-      <c r="D3" s="81">
+      <c r="D3" s="80">
         <v>1.3752</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="58" t="s">
-        <v>397</v>
-      </c>
-      <c r="C4" s="85">
+        <v>396</v>
+      </c>
+      <c r="C4" s="84">
         <v>1.875</v>
       </c>
-      <c r="D4" s="88">
+      <c r="D4" s="87">
         <v>1.125</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="58" t="s">
-        <v>398</v>
-      </c>
-      <c r="C5" s="85">
+        <v>397</v>
+      </c>
+      <c r="C5" s="84">
         <v>6.0625</v>
       </c>
-      <c r="D5" s="88">
+      <c r="D5" s="87">
         <v>4.375</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="58" t="s">
-        <v>399</v>
-      </c>
-      <c r="C6" s="90">
+        <v>398</v>
+      </c>
+      <c r="C6" s="89">
         <v>5</v>
       </c>
-      <c r="D6" s="93">
+      <c r="D6" s="92">
         <v>3.25</v>
       </c>
     </row>
@@ -18359,7 +18358,7 @@
     </row>
     <row r="166" spans="2:9">
       <c r="E166" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F166">
         <f>AVEDEV(H168:H183)</f>
@@ -18375,82 +18374,82 @@
       </c>
     </row>
     <row r="168" spans="2:9">
-      <c r="H168" s="176">
+      <c r="H168" s="158">
         <v>2</v>
       </c>
     </row>
     <row r="169" spans="2:9">
-      <c r="H169" s="176">
+      <c r="H169" s="158">
         <v>2</v>
       </c>
     </row>
     <row r="170" spans="2:9">
-      <c r="H170" s="176">
+      <c r="H170" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="171" spans="2:9">
-      <c r="H171" s="176">
+      <c r="H171" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="172" spans="2:9">
-      <c r="H172" s="176">
+      <c r="H172" s="158">
         <v>2</v>
       </c>
     </row>
     <row r="173" spans="2:9">
-      <c r="H173" s="176">
+      <c r="H173" s="158">
         <v>2</v>
       </c>
     </row>
     <row r="174" spans="2:9">
-      <c r="H174" s="176">
+      <c r="H174" s="158">
         <v>2</v>
       </c>
     </row>
     <row r="175" spans="2:9">
-      <c r="H175" s="176">
+      <c r="H175" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="176" spans="2:9">
-      <c r="H176" s="176">
+      <c r="H176" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="177" spans="8:8">
-      <c r="H177" s="176">
+      <c r="H177" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="178" spans="8:8">
-      <c r="H178" s="176">
+      <c r="H178" s="158">
         <v>2</v>
       </c>
     </row>
     <row r="179" spans="8:8">
-      <c r="H179" s="176">
+      <c r="H179" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="180" spans="8:8">
-      <c r="H180" s="176">
+      <c r="H180" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="181" spans="8:8">
-      <c r="H181" s="176">
+      <c r="H181" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="182" spans="8:8">
-      <c r="H182" s="176">
+      <c r="H182" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="183" spans="8:8">
-      <c r="H183" s="176">
+      <c r="H183" s="158">
         <v>1</v>
       </c>
     </row>
@@ -20990,7 +20989,7 @@
     </row>
     <row r="166" spans="2:9">
       <c r="E166" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F166">
         <f>AVEDEV(H168:H183)</f>
@@ -21009,84 +21008,84 @@
     <row r="168" spans="2:9">
       <c r="E168" s="25"/>
       <c r="G168" s="65"/>
-      <c r="H168" s="175">
+      <c r="H168" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="169" spans="2:9">
       <c r="E169" s="25"/>
       <c r="G169" s="29"/>
-      <c r="H169" s="175">
+      <c r="H169" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="170" spans="2:9">
-      <c r="H170" s="175">
+      <c r="H170" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="171" spans="2:9">
-      <c r="H171" s="175">
+      <c r="H171" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="172" spans="2:9">
-      <c r="H172" s="175">
+      <c r="H172" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="173" spans="2:9">
-      <c r="H173" s="175">
+      <c r="H173" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="174" spans="2:9">
-      <c r="H174" s="175">
+      <c r="H174" s="157">
         <v>5</v>
       </c>
     </row>
     <row r="175" spans="2:9">
-      <c r="H175" s="175">
+      <c r="H175" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="176" spans="2:9">
-      <c r="H176" s="175">
+      <c r="H176" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="177" spans="8:8">
-      <c r="H177" s="175">
+      <c r="H177" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="178" spans="8:8">
-      <c r="H178" s="175">
+      <c r="H178" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="179" spans="8:8">
-      <c r="H179" s="175">
+      <c r="H179" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="180" spans="8:8">
-      <c r="H180" s="175">
+      <c r="H180" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="181" spans="8:8">
-      <c r="H181" s="175">
+      <c r="H181" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="182" spans="8:8">
-      <c r="H182" s="175">
+      <c r="H182" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="183" spans="8:8">
-      <c r="H183" s="175">
+      <c r="H183" s="157">
         <v>2</v>
       </c>
     </row>
@@ -23614,19 +23613,19 @@
       <c r="F165">
         <v>1.125</v>
       </c>
-      <c r="H165" s="176">
+      <c r="H165" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="166" spans="2:9">
       <c r="E166" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F166">
         <f>AVEDEV(H169:H184)</f>
         <v>0.15277777777777771</v>
       </c>
-      <c r="H166" s="176">
+      <c r="H166" s="158">
         <v>2</v>
       </c>
     </row>
@@ -23637,72 +23636,72 @@
       <c r="F167">
         <v>2</v>
       </c>
-      <c r="H167" s="176">
+      <c r="H167" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="168" spans="2:9">
-      <c r="H168" s="176">
+      <c r="H168" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="169" spans="2:9">
-      <c r="H169" s="176">
+      <c r="H169" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="170" spans="2:9">
-      <c r="H170" s="176">
+      <c r="H170" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="171" spans="2:9">
-      <c r="H171" s="176">
+      <c r="H171" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="172" spans="2:9">
-      <c r="H172" s="176">
+      <c r="H172" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="173" spans="2:9">
-      <c r="H173" s="176">
+      <c r="H173" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="174" spans="2:9">
-      <c r="H174" s="176">
+      <c r="H174" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="175" spans="2:9">
-      <c r="H175" s="176">
+      <c r="H175" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="176" spans="2:9">
-      <c r="H176" s="176">
+      <c r="H176" s="158">
         <v>2</v>
       </c>
     </row>
     <row r="177" spans="8:8">
-      <c r="H177" s="176">
+      <c r="H177" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="178" spans="8:8">
-      <c r="H178" s="176">
+      <c r="H178" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="179" spans="8:8">
-      <c r="H179" s="176">
+      <c r="H179" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="180" spans="8:8">
-      <c r="H180" s="176">
+      <c r="H180" s="158">
         <v>1</v>
       </c>
     </row>
@@ -26245,7 +26244,7 @@
     </row>
     <row r="166" spans="2:9">
       <c r="E166" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F166">
         <f>AVEDEV(H169:H184)</f>
@@ -26271,82 +26270,82 @@
     <row r="169" spans="2:9">
       <c r="E169" s="25"/>
       <c r="G169" s="29"/>
-      <c r="H169" s="175">
+      <c r="H169" s="157">
         <v>7</v>
       </c>
     </row>
     <row r="170" spans="2:9">
-      <c r="H170" s="175">
+      <c r="H170" s="157">
         <v>7</v>
       </c>
     </row>
     <row r="171" spans="2:9">
-      <c r="H171" s="175">
+      <c r="H171" s="157">
         <v>6</v>
       </c>
     </row>
     <row r="172" spans="2:9">
-      <c r="H172" s="175">
+      <c r="H172" s="157">
         <v>6</v>
       </c>
     </row>
     <row r="173" spans="2:9">
-      <c r="H173" s="175">
+      <c r="H173" s="157">
         <v>6</v>
       </c>
     </row>
     <row r="174" spans="2:9">
-      <c r="H174" s="175">
+      <c r="H174" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="175" spans="2:9">
-      <c r="H175" s="175">
+      <c r="H175" s="157">
         <v>8</v>
       </c>
     </row>
     <row r="176" spans="2:9">
-      <c r="H176" s="175">
+      <c r="H176" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="177" spans="8:8">
-      <c r="H177" s="175">
+      <c r="H177" s="157">
         <v>5</v>
       </c>
     </row>
     <row r="178" spans="8:8">
-      <c r="H178" s="175">
+      <c r="H178" s="157">
         <v>4</v>
       </c>
     </row>
     <row r="179" spans="8:8">
-      <c r="H179" s="175">
+      <c r="H179" s="157">
         <v>8</v>
       </c>
     </row>
     <row r="180" spans="8:8">
-      <c r="H180" s="175">
+      <c r="H180" s="157">
         <v>9</v>
       </c>
     </row>
     <row r="181" spans="8:8">
-      <c r="H181" s="175">
+      <c r="H181" s="157">
         <v>4</v>
       </c>
     </row>
     <row r="182" spans="8:8">
-      <c r="H182" s="175">
+      <c r="H182" s="157">
         <v>6</v>
       </c>
     </row>
     <row r="183" spans="8:8">
-      <c r="H183" s="175">
+      <c r="H183" s="157">
         <v>8</v>
       </c>
     </row>
     <row r="184" spans="8:8">
-      <c r="H184" s="175">
+      <c r="H184" s="157">
         <v>8</v>
       </c>
     </row>
@@ -28874,19 +28873,19 @@
       <c r="F165">
         <v>1.4375</v>
       </c>
-      <c r="H165" s="176">
+      <c r="H165" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="166" spans="2:9">
       <c r="E166" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F166">
         <f>AVEDEV(H165:H180)</f>
         <v>0.7109375</v>
       </c>
-      <c r="H166" s="176">
+      <c r="H166" s="158">
         <v>2</v>
       </c>
     </row>
@@ -28897,72 +28896,72 @@
       <c r="F167">
         <v>6</v>
       </c>
-      <c r="H167" s="176">
+      <c r="H167" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="168" spans="2:9">
-      <c r="H168" s="176">
+      <c r="H168" s="158">
         <v>6</v>
       </c>
     </row>
     <row r="169" spans="2:9">
-      <c r="H169" s="176">
+      <c r="H169" s="158">
         <v>2</v>
       </c>
     </row>
     <row r="170" spans="2:9">
-      <c r="H170" s="176">
+      <c r="H170" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="171" spans="2:9">
-      <c r="H171" s="176">
+      <c r="H171" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="172" spans="2:9">
-      <c r="H172" s="176">
+      <c r="H172" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="173" spans="2:9">
-      <c r="H173" s="176">
+      <c r="H173" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="174" spans="2:9">
-      <c r="H174" s="176">
+      <c r="H174" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="175" spans="2:9">
-      <c r="H175" s="176">
+      <c r="H175" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="176" spans="2:9">
-      <c r="H176" s="176">
+      <c r="H176" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="177" spans="8:8">
-      <c r="H177" s="176">
+      <c r="H177" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="178" spans="8:8">
-      <c r="H178" s="176">
+      <c r="H178" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="179" spans="8:8">
-      <c r="H179" s="176">
+      <c r="H179" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="180" spans="8:8">
-      <c r="H180" s="176">
+      <c r="H180" s="158">
         <v>1</v>
       </c>
     </row>
@@ -31502,7 +31501,7 @@
     </row>
     <row r="166" spans="2:9">
       <c r="E166" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F166">
         <f>AVEDEV(H168:H183)</f>
@@ -31521,84 +31520,84 @@
     <row r="168" spans="2:9">
       <c r="E168" s="25"/>
       <c r="G168" s="65"/>
-      <c r="H168" s="175">
+      <c r="H168" s="157">
         <v>4</v>
       </c>
     </row>
     <row r="169" spans="2:9">
       <c r="E169" s="25"/>
       <c r="G169" s="29"/>
-      <c r="H169" s="175">
+      <c r="H169" s="157">
         <v>4</v>
       </c>
     </row>
     <row r="170" spans="2:9">
-      <c r="H170" s="175">
+      <c r="H170" s="157">
         <v>6</v>
       </c>
     </row>
     <row r="171" spans="2:9">
-      <c r="H171" s="175">
+      <c r="H171" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="172" spans="2:9">
-      <c r="H172" s="175">
+      <c r="H172" s="157">
         <v>10</v>
       </c>
     </row>
     <row r="173" spans="2:9">
-      <c r="H173" s="175">
+      <c r="H173" s="157">
         <v>7</v>
       </c>
     </row>
     <row r="174" spans="2:9">
-      <c r="H174" s="175">
+      <c r="H174" s="157">
         <v>7</v>
       </c>
     </row>
     <row r="175" spans="2:9">
-      <c r="H175" s="175">
+      <c r="H175" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="176" spans="2:9">
-      <c r="H176" s="175">
+      <c r="H176" s="157">
         <v>4</v>
       </c>
     </row>
     <row r="177" spans="8:8">
-      <c r="H177" s="175">
+      <c r="H177" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="178" spans="8:8">
-      <c r="H178" s="175">
+      <c r="H178" s="157">
         <v>9</v>
       </c>
     </row>
     <row r="179" spans="8:8">
-      <c r="H179" s="175">
+      <c r="H179" s="157">
         <v>5</v>
       </c>
     </row>
     <row r="180" spans="8:8">
-      <c r="H180" s="175">
+      <c r="H180" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="181" spans="8:8">
-      <c r="H181" s="175">
+      <c r="H181" s="157">
         <v>4</v>
       </c>
     </row>
     <row r="182" spans="8:8">
-      <c r="H182" s="175">
+      <c r="H182" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="183" spans="8:8">
-      <c r="H183" s="175">
+      <c r="H183" s="157">
         <v>6</v>
       </c>
     </row>
@@ -34129,13 +34128,13 @@
     </row>
     <row r="166" spans="2:9">
       <c r="E166" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F166">
         <f>AVEDEV(H166:H181)</f>
         <v>1.96875</v>
       </c>
-      <c r="H166" s="176">
+      <c r="H166" s="158">
         <v>3</v>
       </c>
     </row>
@@ -34146,77 +34145,77 @@
       <c r="F167">
         <v>8</v>
       </c>
-      <c r="H167" s="176">
+      <c r="H167" s="158">
         <v>5</v>
       </c>
     </row>
     <row r="168" spans="2:9">
-      <c r="H168" s="176">
+      <c r="H168" s="158">
         <v>3</v>
       </c>
     </row>
     <row r="169" spans="2:9">
-      <c r="H169" s="176">
+      <c r="H169" s="158">
         <v>7</v>
       </c>
     </row>
     <row r="170" spans="2:9">
-      <c r="H170" s="176">
+      <c r="H170" s="158">
         <v>7</v>
       </c>
     </row>
     <row r="171" spans="2:9">
-      <c r="H171" s="176">
+      <c r="H171" s="158">
         <v>3</v>
       </c>
     </row>
     <row r="172" spans="2:9">
-      <c r="H172" s="176">
+      <c r="H172" s="158">
         <v>8</v>
       </c>
     </row>
     <row r="173" spans="2:9">
-      <c r="H173" s="176">
+      <c r="H173" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="174" spans="2:9">
-      <c r="H174" s="176">
+      <c r="H174" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="175" spans="2:9">
-      <c r="H175" s="176">
+      <c r="H175" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="176" spans="2:9">
-      <c r="H176" s="176">
+      <c r="H176" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="177" spans="8:8">
-      <c r="H177" s="176">
+      <c r="H177" s="158">
         <v>2</v>
       </c>
     </row>
     <row r="178" spans="8:8">
-      <c r="H178" s="176">
+      <c r="H178" s="158">
         <v>5</v>
       </c>
     </row>
     <row r="179" spans="8:8">
-      <c r="H179" s="176">
+      <c r="H179" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="180" spans="8:8">
-      <c r="H180" s="176">
+      <c r="H180" s="158">
         <v>3</v>
       </c>
     </row>
     <row r="181" spans="8:8">
-      <c r="H181" s="178">
+      <c r="H181" s="160">
         <v>1</v>
       </c>
     </row>
@@ -36756,7 +36755,7 @@
     </row>
     <row r="166" spans="2:9">
       <c r="E166" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F166">
         <f>AVEDEV(H169:H184)</f>
@@ -36775,82 +36774,82 @@
       </c>
     </row>
     <row r="169" spans="2:9">
-      <c r="H169" s="175">
+      <c r="H169" s="157">
         <v>4</v>
       </c>
     </row>
     <row r="170" spans="2:9">
-      <c r="H170" s="175">
+      <c r="H170" s="157">
         <v>4</v>
       </c>
     </row>
     <row r="171" spans="2:9">
-      <c r="H171" s="175">
+      <c r="H171" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="172" spans="2:9">
-      <c r="H172" s="175">
+      <c r="H172" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="173" spans="2:9">
-      <c r="H173" s="175">
+      <c r="H173" s="157">
         <v>6</v>
       </c>
     </row>
     <row r="174" spans="2:9">
-      <c r="H174" s="175">
+      <c r="H174" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="175" spans="2:9">
-      <c r="H175" s="175">
+      <c r="H175" s="157">
         <v>6</v>
       </c>
     </row>
     <row r="176" spans="2:9">
-      <c r="H176" s="175">
+      <c r="H176" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="177" spans="8:8">
-      <c r="H177" s="175">
+      <c r="H177" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="178" spans="8:8">
-      <c r="H178" s="175">
+      <c r="H178" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="179" spans="8:8">
-      <c r="H179" s="175">
+      <c r="H179" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="180" spans="8:8">
-      <c r="H180" s="175">
+      <c r="H180" s="157">
         <v>3</v>
       </c>
     </row>
     <row r="181" spans="8:8">
-      <c r="H181" s="175">
+      <c r="H181" s="157">
         <v>4</v>
       </c>
     </row>
     <row r="182" spans="8:8">
-      <c r="H182" s="175">
+      <c r="H182" s="157">
         <v>1</v>
       </c>
     </row>
     <row r="183" spans="8:8">
-      <c r="H183" s="175">
+      <c r="H183" s="157">
         <v>2</v>
       </c>
     </row>
     <row r="184" spans="8:8">
-      <c r="H184" s="175">
+      <c r="H184" s="157">
         <v>3</v>
       </c>
     </row>

</xml_diff>